<commit_message>
added personal auto methods
</commit_message>
<xml_diff>
--- a/CucumberTest/src/TestData/AutoTestData.xlsx
+++ b/CucumberTest/src/TestData/AutoTestData.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27031"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adragutinovic\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NastasjaDamjanac\Desktop\SandboxAutomation\Sandbox-Automation\CucumberTest\src\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2BB287B6-2768-4307-ABB6-213EF3D7C98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8D92654-34C2-4950-B057-5AD367FCD71F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F560B6A-2F60-4AE5-9DCC-8EAA7648F486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D341BFEF-FEF1-4343-8272-FBF06FB03C18}"/>
+    <workbookView xWindow="28695" yWindow="7740" windowWidth="29010" windowHeight="7845" activeTab="2" xr2:uid="{D341BFEF-FEF1-4343-8272-FBF06FB03C18}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="HomePage" sheetId="5" r:id="rId1"/>
+    <sheet name="CustomerData" sheetId="4" r:id="rId2"/>
+    <sheet name="PersonalAutoData" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="285">
   <si>
     <t>Program</t>
   </si>
@@ -44,9 +46,6 @@
     <t>Billing Method</t>
   </si>
   <si>
-    <t xml:space="preserve">Has anyone knowingly provided material </t>
-  </si>
-  <si>
     <t>Does any vehicle have any existing damage?</t>
   </si>
   <si>
@@ -366,13 +365,541 @@
   </si>
   <si>
     <t>Contractor</t>
+  </si>
+  <si>
+    <t>Braintree</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>02184</t>
+  </si>
+  <si>
+    <t>773Granite St</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>test20@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4121</t>
+  </si>
+  <si>
+    <t>3/29/1943</t>
+  </si>
+  <si>
+    <t>Burns</t>
+  </si>
+  <si>
+    <t>Frederick</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>Bourne</t>
+  </si>
+  <si>
+    <t>02532</t>
+  </si>
+  <si>
+    <t>23Waterhouse Rd</t>
+  </si>
+  <si>
+    <t>test19@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4120</t>
+  </si>
+  <si>
+    <t>5/15/1949</t>
+  </si>
+  <si>
+    <t>Casey</t>
+  </si>
+  <si>
+    <t>Craig</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>02127</t>
+  </si>
+  <si>
+    <t>593E 4Th St</t>
+  </si>
+  <si>
+    <t>test18@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4119</t>
+  </si>
+  <si>
+    <t>10/9/1970</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Vonda</t>
+  </si>
+  <si>
+    <t>894E 2Nd St</t>
+  </si>
+  <si>
+    <t>test17@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4118</t>
+  </si>
+  <si>
+    <t>1/4/1950</t>
+  </si>
+  <si>
+    <t>Blakemore</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>02116</t>
+  </si>
+  <si>
+    <t>27Braddock Park</t>
+  </si>
+  <si>
+    <t>test16@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4117</t>
+  </si>
+  <si>
+    <t>12/26/1961</t>
+  </si>
+  <si>
+    <t>Ooms</t>
+  </si>
+  <si>
+    <t>Desiree</t>
+  </si>
+  <si>
+    <t>106Appleton St</t>
+  </si>
+  <si>
+    <t>test15@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4116</t>
+  </si>
+  <si>
+    <t>12/22/1950</t>
+  </si>
+  <si>
+    <t>Gelding</t>
+  </si>
+  <si>
+    <t>Theresa</t>
+  </si>
+  <si>
+    <t>02130</t>
+  </si>
+  <si>
+    <t>107Chestnut Ave</t>
+  </si>
+  <si>
+    <t>test14@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4115</t>
+  </si>
+  <si>
+    <t>2/1/1955</t>
+  </si>
+  <si>
+    <t>Brumback</t>
+  </si>
+  <si>
+    <t>Sandra</t>
+  </si>
+  <si>
+    <t>Billerica</t>
+  </si>
+  <si>
+    <t>01821</t>
+  </si>
+  <si>
+    <t>5Griffin Cir</t>
+  </si>
+  <si>
+    <t>test13@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4114</t>
+  </si>
+  <si>
+    <t>11/12/1970</t>
+  </si>
+  <si>
+    <t>Dugger</t>
+  </si>
+  <si>
+    <t>Linda</t>
+  </si>
+  <si>
+    <t>26Ernest Rd</t>
+  </si>
+  <si>
+    <t>test12@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4113</t>
+  </si>
+  <si>
+    <t>11/2/1970</t>
+  </si>
+  <si>
+    <t>Fierros</t>
+  </si>
+  <si>
+    <t>Lori</t>
+  </si>
+  <si>
+    <t>Belmont</t>
+  </si>
+  <si>
+    <t>02478</t>
+  </si>
+  <si>
+    <t>44Hill Rd</t>
+  </si>
+  <si>
+    <t>test11@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4112</t>
+  </si>
+  <si>
+    <t>5/15/1955</t>
+  </si>
+  <si>
+    <t>Bailey</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>26Beatrice Cir</t>
+  </si>
+  <si>
+    <t>test10@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4111</t>
+  </si>
+  <si>
+    <t>12/9/1944</t>
+  </si>
+  <si>
+    <t>Richards</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Arlington</t>
+  </si>
+  <si>
+    <t>02476</t>
+  </si>
+  <si>
+    <t>110Gray St</t>
+  </si>
+  <si>
+    <t>test9@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4110</t>
+  </si>
+  <si>
+    <t>12/25/1950</t>
+  </si>
+  <si>
+    <t>Eccles</t>
+  </si>
+  <si>
+    <t>Tracy</t>
+  </si>
+  <si>
+    <t>14Bailey Rd</t>
+  </si>
+  <si>
+    <t>test8@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4109</t>
+  </si>
+  <si>
+    <t>9/8/1957</t>
+  </si>
+  <si>
+    <t>Sanchez</t>
+  </si>
+  <si>
+    <t>Pam</t>
+  </si>
+  <si>
+    <t>02474</t>
+  </si>
+  <si>
+    <t>57James St</t>
+  </si>
+  <si>
+    <t>test7@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4108</t>
+  </si>
+  <si>
+    <t>11/1/1948</t>
+  </si>
+  <si>
+    <t>Parks</t>
+  </si>
+  <si>
+    <t>Jacqueli</t>
+  </si>
+  <si>
+    <t>Andover</t>
+  </si>
+  <si>
+    <t>01810</t>
+  </si>
+  <si>
+    <t>4Barron Ct</t>
+  </si>
+  <si>
+    <t>test6@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4107</t>
+  </si>
+  <si>
+    <t>10/17/1959</t>
+  </si>
+  <si>
+    <t>Bristow</t>
+  </si>
+  <si>
+    <t>Odell</t>
+  </si>
+  <si>
+    <t>Abington</t>
+  </si>
+  <si>
+    <t>02351</t>
+  </si>
+  <si>
+    <t>96Hamilton St</t>
+  </si>
+  <si>
+    <t>test5@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4106</t>
+  </si>
+  <si>
+    <t>2/13/1951</t>
+  </si>
+  <si>
+    <t>Blakely</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>617Plymouth St</t>
+  </si>
+  <si>
+    <t>test4@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4105</t>
+  </si>
+  <si>
+    <t>2/10/1923</t>
+  </si>
+  <si>
+    <t>Macleod</t>
+  </si>
+  <si>
+    <t>188Oak St</t>
+  </si>
+  <si>
+    <t>test3@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4104</t>
+  </si>
+  <si>
+    <t>6/26/1956</t>
+  </si>
+  <si>
+    <t>Brigandi</t>
+  </si>
+  <si>
+    <t>Blanche</t>
+  </si>
+  <si>
+    <t>204Helen Dr</t>
+  </si>
+  <si>
+    <t>test2@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4103</t>
+  </si>
+  <si>
+    <t>3/6/1962</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Fall River</t>
+  </si>
+  <si>
+    <t>02720</t>
+  </si>
+  <si>
+    <t>353 Archer St</t>
+  </si>
+  <si>
+    <t>test1@test.com</t>
+  </si>
+  <si>
+    <t>(125)-896-4102</t>
+  </si>
+  <si>
+    <t>10/10/1975</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Address Line 2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>ZIP Code</t>
+  </si>
+  <si>
+    <t>Address Line 1</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>FEIN</t>
+  </si>
+  <si>
+    <t>Establishment Date</t>
+  </si>
+  <si>
+    <t>Doing Business As</t>
+  </si>
+  <si>
+    <t>Business Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>Customer Type</t>
+  </si>
+  <si>
+    <t>Submission Type</t>
+  </si>
+  <si>
+    <t>Producer</t>
+  </si>
+  <si>
+    <t>Effective Date</t>
+  </si>
+  <si>
+    <t>Inception Date</t>
+  </si>
+  <si>
+    <t>Prior Policy Number</t>
+  </si>
+  <si>
+    <t>New Business</t>
+  </si>
+  <si>
+    <t>Janis Irey</t>
+  </si>
+  <si>
+    <t>10/23/2023</t>
+  </si>
+  <si>
+    <t>Renewal</t>
+  </si>
+  <si>
+    <t>10/24/2023</t>
+  </si>
+  <si>
+    <t>05/20/2000</t>
+  </si>
+  <si>
+    <t>10/30/2023</t>
+  </si>
+  <si>
+    <t>Homeowner</t>
+  </si>
+  <si>
+    <t>10/24/2021</t>
+  </si>
+  <si>
+    <t>10/10/2000</t>
+  </si>
+  <si>
+    <t>10/24/2022</t>
+  </si>
+  <si>
+    <t>Has anyone knowingly provided material</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -386,8 +913,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,8 +941,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -489,11 +1036,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -503,8 +1124,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -816,40 +1448,1377 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6869B195-6779-4655-B0FD-10114DB2FCAC}">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="13.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C167A2-CD5C-4977-B794-BF3104AB0DCB}">
+  <dimension ref="A1:P21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="10" width="18.109375" customWidth="1"/>
+    <col min="11" max="12" width="17.109375" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="P2" s="6"/>
+    </row>
+    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" t="s">
+        <v>236</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P21" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{723BF622-639C-445E-86D8-65F4F3BFC966}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{37966D14-B0D4-4D3F-B9BD-327ACA7B2ABB}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{5F6E83C4-6A94-4B51-B42E-4E3A70121F6F}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{50AE7F2C-2163-43BD-A7C5-4A84667F6A53}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{3268AC34-99CE-4469-A1E8-145136FA2A62}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{3B80D97F-A6E9-43B1-9B6C-E06E84C40428}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{2F40C7A6-7D81-4AF2-89CD-E3D4E288C7C5}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{98C6CE47-2A90-4CB9-98D7-770BB2CB22E0}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{7F8353C7-BF3C-4030-8F48-75680032F838}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{89CBC2EF-4CCF-43A2-A462-FD96F67A46BE}"/>
+    <hyperlink ref="F12:F21" r:id="rId11" display="test10@test.com" xr:uid="{692879E0-D922-4433-ACED-C10631B80F70}"/>
+    <hyperlink ref="F12" r:id="rId12" xr:uid="{13B90B2B-571A-46AC-A2F5-E2EA9DC58668}"/>
+    <hyperlink ref="F13" r:id="rId13" xr:uid="{25A4BEE1-9AA1-42E6-9B11-F762AF160726}"/>
+    <hyperlink ref="F14" r:id="rId14" xr:uid="{29568F8B-FCD4-464A-A2AF-DD22FA67AE53}"/>
+    <hyperlink ref="F15" r:id="rId15" xr:uid="{F4734191-7ADA-4D40-A375-1D9D55C74DDA}"/>
+    <hyperlink ref="F16" r:id="rId16" xr:uid="{6CB3D35D-CB18-45D6-B314-16CC7FF103F6}"/>
+    <hyperlink ref="F17" r:id="rId17" xr:uid="{9B258891-D149-45A7-94A2-9B886B07C9EF}"/>
+    <hyperlink ref="F18" r:id="rId18" xr:uid="{49D5865A-C9F5-4270-A4ED-62D3EAC97E4A}"/>
+    <hyperlink ref="F19" r:id="rId19" xr:uid="{78E79EEF-50EA-4289-A2E1-66F14E695AAF}"/>
+    <hyperlink ref="F20" r:id="rId20" xr:uid="{F159972E-3163-4467-BBCF-3C0BC0442581}"/>
+    <hyperlink ref="F21" r:id="rId21" xr:uid="{00F6B3F4-9C95-41D0-8F89-517F4CE657DA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E20C209-DAE8-4732-ABB1-5932DEEC5404}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Y7" sqref="Y7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" customWidth="1"/>
-    <col min="11" max="11" width="28.42578125" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
-    <col min="15" max="15" width="53.7109375" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" customWidth="1"/>
-    <col min="17" max="17" width="21.42578125" customWidth="1"/>
-    <col min="18" max="18" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" customWidth="1"/>
+    <col min="1" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" customWidth="1"/>
+    <col min="10" max="10" width="18.109375" customWidth="1"/>
+    <col min="11" max="11" width="28.44140625" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" customWidth="1"/>
+    <col min="15" max="15" width="53.6640625" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" customWidth="1"/>
+    <col min="17" max="17" width="21.44140625" customWidth="1"/>
+    <col min="18" max="18" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" customWidth="1"/>
     <col min="20" max="20" width="31" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.42578125" customWidth="1"/>
-    <col min="23" max="23" width="11.140625" customWidth="1"/>
-    <col min="24" max="24" width="12.7109375" customWidth="1"/>
-    <col min="25" max="25" width="15.42578125" customWidth="1"/>
+    <col min="21" max="21" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.44140625" customWidth="1"/>
+    <col min="23" max="23" width="11.109375" customWidth="1"/>
+    <col min="24" max="24" width="12.6640625" customWidth="1"/>
+    <col min="25" max="25" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -857,141 +2826,141 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:25">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="I2" s="3">
         <v>1999</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="L2" s="3">
         <v>2017</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="W2" s="1">
         <v>25000</v>
@@ -1003,72 +2972,72 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="I3" s="3">
         <v>2000</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L3" s="3">
         <v>2017</v>
       </c>
       <c r="M3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="U3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W3" s="1">
         <v>25000</v>
@@ -1080,72 +3049,72 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="I4" s="3">
         <v>2001</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L4" s="1">
         <v>2017</v>
       </c>
       <c r="M4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="O4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T4" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="R4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="U4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W4" s="1">
         <v>25000</v>
@@ -1157,72 +3126,72 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="I5" s="3">
         <v>2002</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L5" s="1">
         <v>2018</v>
       </c>
       <c r="M5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="O5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T5" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="U5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W5" s="1">
         <v>25000</v>
@@ -1234,72 +3203,72 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="I6" s="3">
         <v>2003</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L6" s="1">
         <v>2018</v>
       </c>
       <c r="M6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N6" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="O6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T6" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="R6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="U6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W6" s="1">
         <v>25000</v>
@@ -1311,72 +3280,72 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I7" s="3">
         <v>2004</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L7" s="1">
         <v>2018</v>
       </c>
       <c r="M7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="O7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T7" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="R7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="S7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="V7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W7" s="1">
         <v>25000</v>
@@ -1388,72 +3357,72 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" s="3">
         <v>2005</v>
       </c>
       <c r="J8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="L8" s="1">
         <v>2018</v>
       </c>
       <c r="M8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N8" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="O8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T8" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="R8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="S8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T8" s="1" t="s">
+      <c r="V8" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="W8" s="1">
         <v>25000</v>
@@ -1465,72 +3434,72 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" s="3">
         <v>2006</v>
       </c>
       <c r="J9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="L9" s="1">
         <v>2019</v>
       </c>
       <c r="M9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N9" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="O9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="P9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="R9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="S9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="V9" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="W9" s="1">
         <v>25000</v>
@@ -1542,72 +3511,72 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I10" s="3">
         <v>2007</v>
       </c>
       <c r="J10" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="L10" s="1">
         <v>2019</v>
       </c>
       <c r="M10" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="N10" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="N10" s="6" t="s">
+      <c r="O10" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="P10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q10" s="1" t="s">
+      <c r="R10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="S10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T10" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="W10" s="1">
         <v>25000</v>
@@ -1619,72 +3588,72 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I11" s="3">
         <v>2008</v>
       </c>
       <c r="J11" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="L11" s="1">
         <v>2019</v>
       </c>
       <c r="M11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="N11" s="6" t="s">
+      <c r="O11" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="P11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T11" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="P11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="R11" s="1" t="s">
+      <c r="U11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="S11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T11" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="V11" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="W11" s="1">
         <v>25000</v>
@@ -1699,5 +3668,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Auto smoke and added Auto regression methods
</commit_message>
<xml_diff>
--- a/CucumberTest/src/TestData/AutoTestData.xlsx
+++ b/CucumberTest/src/TestData/AutoTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NastasjaDamjanac\Desktop\SandboxAutomation\Sandbox-Automation\CucumberTest\src\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adragutinovic\Desktop\Projekti\Sandbox-Automation\CucumberTest\src\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F560B6A-2F60-4AE5-9DCC-8EAA7648F486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F939A2B-257D-4F73-943D-B05C820027B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="7740" windowWidth="29010" windowHeight="7845" activeTab="2" xr2:uid="{D341BFEF-FEF1-4343-8272-FBF06FB03C18}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{D341BFEF-FEF1-4343-8272-FBF06FB03C18}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="308">
   <si>
     <t>Program</t>
   </si>
@@ -763,9 +763,6 @@
     <t>(125)-896-4103</t>
   </si>
   <si>
-    <t>3/6/1962</t>
-  </si>
-  <si>
     <t>Miller</t>
   </si>
   <si>
@@ -893,6 +890,78 @@
   </si>
   <si>
     <t>Has anyone knowingly provided material</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>3/6/1982</t>
+  </si>
+  <si>
+    <t>Incident Date</t>
+  </si>
+  <si>
+    <t>10/10/1999</t>
+  </si>
+  <si>
+    <t>10/10/2001</t>
+  </si>
+  <si>
+    <t>10/10/2002</t>
+  </si>
+  <si>
+    <t>10/10/2003</t>
+  </si>
+  <si>
+    <t>10/10/2004</t>
+  </si>
+  <si>
+    <t>10/10/2005</t>
+  </si>
+  <si>
+    <t>10/10/2006</t>
+  </si>
+  <si>
+    <t>10/10/2007</t>
+  </si>
+  <si>
+    <t>10/10/2008</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1183,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1134,6 +1203,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1468,25 +1541,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>269</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>270</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>271</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1494,13 +1567,13 @@
         <v>110</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="11" t="s">
         <v>274</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>275</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>24</v>
@@ -1513,19 +1586,19 @@
         <v>110</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>276</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>277</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -1534,16 +1607,16 @@
         <v>110</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="D4" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1553,19 +1626,19 @@
         <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D5" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>281</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>282</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1574,16 +1647,16 @@
         <v>110</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="D6" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1593,16 +1666,16 @@
         <v>110</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="D7" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1612,16 +1685,16 @@
         <v>110</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="D8" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -1631,16 +1704,16 @@
         <v>110</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="D9" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1650,16 +1723,16 @@
         <v>110</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="D10" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1669,16 +1742,16 @@
         <v>110</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="D11" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1688,16 +1761,16 @@
         <v>110</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="D12" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1707,16 +1780,16 @@
         <v>110</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="D13" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1726,19 +1799,19 @@
         <v>110</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>276</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>277</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1747,13 +1820,13 @@
         <v>110</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="D15" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>24</v>
@@ -1766,13 +1839,13 @@
         <v>110</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="D16" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>24</v>
@@ -1785,19 +1858,19 @@
         <v>110</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>276</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>277</v>
-      </c>
       <c r="E17" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -1806,13 +1879,13 @@
         <v>110</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="D18" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>24</v>
@@ -1825,13 +1898,13 @@
         <v>110</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="D19" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>24</v>
@@ -1844,19 +1917,19 @@
         <v>110</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D20" s="13" t="s">
         <v>276</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>277</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -1865,13 +1938,13 @@
         <v>110</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="D21" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>24</v>
@@ -1889,7 +1962,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P21"/>
+      <selection activeCell="D2" sqref="D2:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1908,52 +1981,52 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L1" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P1" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1961,19 +2034,19 @@
         <v>119</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1983,16 +2056,16 @@
         <v>113</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>110</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P2" s="6"/>
     </row>
@@ -2001,13 +2074,13 @@
         <v>119</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>241</v>
+        <v>297</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>240</v>
@@ -2786,10 +2859,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E20C209-DAE8-4732-ABB1-5932DEEC5404}">
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2804,6 +2877,7 @@
     <col min="9" max="9" width="12.109375" customWidth="1"/>
     <col min="10" max="10" width="18.109375" customWidth="1"/>
     <col min="11" max="11" width="28.44140625" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="21"/>
     <col min="14" max="14" width="19.6640625" customWidth="1"/>
     <col min="15" max="15" width="53.6640625" customWidth="1"/>
     <col min="16" max="16" width="15.33203125" customWidth="1"/>
@@ -2815,10 +2889,10 @@
     <col min="22" max="22" width="10.44140625" customWidth="1"/>
     <col min="23" max="23" width="11.109375" customWidth="1"/>
     <col min="24" max="24" width="12.6640625" customWidth="1"/>
-    <col min="25" max="25" width="15.44140625" customWidth="1"/>
+    <col min="25" max="26" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2826,7 +2900,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -2852,7 +2926,7 @@
       <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="19" t="s">
         <v>10</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -2894,8 +2968,11 @@
       <c r="Y1" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z1" s="22" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -2920,8 +2997,8 @@
       <c r="H2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="3">
-        <v>1999</v>
+      <c r="I2" s="3" t="s">
+        <v>284</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>31</v>
@@ -2929,8 +3006,8 @@
       <c r="K2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="3">
-        <v>2017</v>
+      <c r="L2" s="20" t="s">
+        <v>294</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>33</v>
@@ -2971,8 +3048,11 @@
       <c r="Y2" s="6">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z2" s="13" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -2997,8 +3077,8 @@
       <c r="H3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="3">
-        <v>2000</v>
+      <c r="I3" s="3" t="s">
+        <v>285</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>42</v>
@@ -3006,8 +3086,8 @@
       <c r="K3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="3">
-        <v>2017</v>
+      <c r="L3" s="20" t="s">
+        <v>294</v>
       </c>
       <c r="M3" t="s">
         <v>43</v>
@@ -3048,8 +3128,11 @@
       <c r="Y3" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z3" s="13" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -3074,8 +3157,8 @@
       <c r="H4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="3">
-        <v>2001</v>
+      <c r="I4" s="3" t="s">
+        <v>286</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>49</v>
@@ -3083,8 +3166,8 @@
       <c r="K4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="1">
-        <v>2017</v>
+      <c r="L4" s="20" t="s">
+        <v>294</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>50</v>
@@ -3125,8 +3208,11 @@
       <c r="Y4" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z4" s="13" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -3151,8 +3237,8 @@
       <c r="H5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="3">
-        <v>2002</v>
+      <c r="I5" s="3" t="s">
+        <v>287</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>56</v>
@@ -3160,8 +3246,8 @@
       <c r="K5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="1">
-        <v>2018</v>
+      <c r="L5" s="20" t="s">
+        <v>295</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>57</v>
@@ -3202,8 +3288,11 @@
       <c r="Y5" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z5" s="13" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -3228,8 +3317,8 @@
       <c r="H6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="3">
-        <v>2003</v>
+      <c r="I6" s="3" t="s">
+        <v>288</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>63</v>
@@ -3237,8 +3326,8 @@
       <c r="K6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="1">
-        <v>2018</v>
+      <c r="L6" s="20" t="s">
+        <v>295</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>64</v>
@@ -3279,8 +3368,11 @@
       <c r="Y6" s="6">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z6" s="13" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -3305,8 +3397,8 @@
       <c r="H7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="3">
-        <v>2004</v>
+      <c r="I7" s="3" t="s">
+        <v>289</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>71</v>
@@ -3314,8 +3406,8 @@
       <c r="K7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="1">
-        <v>2018</v>
+      <c r="L7" s="20" t="s">
+        <v>295</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>72</v>
@@ -3356,8 +3448,11 @@
       <c r="Y7" s="6">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z7" s="13" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -3382,8 +3477,8 @@
       <c r="H8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="3">
-        <v>2005</v>
+      <c r="I8" s="3" t="s">
+        <v>290</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>78</v>
@@ -3391,8 +3486,8 @@
       <c r="K8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="L8" s="1">
-        <v>2018</v>
+      <c r="L8" s="20" t="s">
+        <v>295</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>80</v>
@@ -3433,8 +3528,11 @@
       <c r="Y8" s="4">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z8" s="13" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -3459,8 +3557,8 @@
       <c r="H9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="3">
-        <v>2006</v>
+      <c r="I9" s="3" t="s">
+        <v>291</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>86</v>
@@ -3468,8 +3566,8 @@
       <c r="K9" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="L9" s="1">
-        <v>2019</v>
+      <c r="L9" s="20" t="s">
+        <v>296</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>88</v>
@@ -3510,8 +3608,11 @@
       <c r="Y9" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z9" s="13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -3536,8 +3637,8 @@
       <c r="H10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="3">
-        <v>2007</v>
+      <c r="I10" s="3" t="s">
+        <v>292</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>94</v>
@@ -3545,8 +3646,8 @@
       <c r="K10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="L10" s="1">
-        <v>2019</v>
+      <c r="L10" s="20" t="s">
+        <v>296</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>96</v>
@@ -3587,8 +3688,11 @@
       <c r="Y10" s="6">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z10" s="13" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -3613,8 +3717,8 @@
       <c r="H11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="3">
-        <v>2008</v>
+      <c r="I11" s="3" t="s">
+        <v>293</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>103</v>
@@ -3622,8 +3726,8 @@
       <c r="K11" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="L11" s="1">
-        <v>2019</v>
+      <c r="L11" s="20" t="s">
+        <v>296</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>105</v>
@@ -3663,6 +3767,9 @@
       </c>
       <c r="Y11" s="1">
         <v>25</v>
+      </c>
+      <c r="Z11" s="13" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Auto smoke and regression
</commit_message>
<xml_diff>
--- a/CucumberTest/src/TestData/AutoTestData.xlsx
+++ b/CucumberTest/src/TestData/AutoTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adragutinovic\Desktop\Projekti\Sandbox-Automation\CucumberTest\src\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F939A2B-257D-4F73-943D-B05C820027B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6ED184F-A25A-499C-A514-6E402083CB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{D341BFEF-FEF1-4343-8272-FBF06FB03C18}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="313">
   <si>
     <t>Program</t>
   </si>
@@ -67,9 +67,6 @@
     <t>License Number</t>
   </si>
   <si>
-    <t>Vechicle Type</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -962,6 +959,24 @@
   </si>
   <si>
     <t>10/10/2008</t>
+  </si>
+  <si>
+    <t>Make2</t>
+  </si>
+  <si>
+    <t>Model2</t>
+  </si>
+  <si>
+    <t>Specification2</t>
+  </si>
+  <si>
+    <t>Vehicle Use2</t>
+  </si>
+  <si>
+    <t>Vehicle Type</t>
+  </si>
+  <si>
+    <t>Ownership2</t>
   </si>
 </sst>
 </file>
@@ -1541,413 +1556,413 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>268</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>269</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>270</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>274</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>276</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>277</v>
       </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="D4" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>279</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D5" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>280</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>281</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="D6" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="D7" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="D8" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="D9" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="D10" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="D11" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="D12" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="D13" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D14" s="13" t="s">
+      <c r="E14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>276</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>277</v>
       </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="D15" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="D16" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>276</v>
-      </c>
       <c r="E17" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="D18" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="D19" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D20" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>276</v>
-      </c>
       <c r="E20" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="D21" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1981,850 +1996,850 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L1" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="P1" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P2" s="6"/>
     </row>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P18" s="1"/>
     </row>
     <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P19" s="1"/>
     </row>
     <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P20" s="1"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P21" s="1"/>
     </row>
@@ -2859,10 +2874,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E20C209-DAE8-4732-ABB1-5932DEEC5404}">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:AE12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2890,9 +2905,13 @@
     <col min="23" max="23" width="11.109375" customWidth="1"/>
     <col min="24" max="24" width="12.6640625" customWidth="1"/>
     <col min="25" max="26" width="15.44140625" customWidth="1"/>
+    <col min="28" max="28" width="19.6640625" customWidth="1"/>
+    <col min="29" max="29" width="53.6640625" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" customWidth="1"/>
+    <col min="31" max="31" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2900,7 +2919,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -2924,120 +2943,135 @@
         <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="L1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="22" t="s">
+        <v>297</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="22" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="W2" s="1">
         <v>25000</v>
@@ -3049,75 +3083,90 @@
         <v>25</v>
       </c>
       <c r="Z2" s="13" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="I3" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="M3" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="N3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="U3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W3" s="1">
         <v>25000</v>
@@ -3129,75 +3178,90 @@
         <v>25</v>
       </c>
       <c r="Z3" s="13" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="O4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="R4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="U4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W4" s="1">
         <v>25000</v>
@@ -3209,75 +3273,90 @@
         <v>25</v>
       </c>
       <c r="Z4" s="13" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+        <v>299</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="I5" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L5" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="O5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="U5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W5" s="1">
         <v>25000</v>
@@ -3289,75 +3368,90 @@
         <v>25</v>
       </c>
       <c r="Z5" s="13" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="O6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T6" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="R6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="U6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W6" s="1">
         <v>25000</v>
@@ -3369,75 +3463,90 @@
         <v>25</v>
       </c>
       <c r="Z6" s="13" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L7" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="O7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T7" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="R7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="S7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="V7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W7" s="1">
         <v>25000</v>
@@ -3449,75 +3558,90 @@
         <v>25</v>
       </c>
       <c r="Z7" s="13" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB7" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="L8" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="O8" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="R8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="S8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T8" s="1" t="s">
+      <c r="V8" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="W8" s="1">
         <v>25000</v>
@@ -3529,75 +3653,90 @@
         <v>25</v>
       </c>
       <c r="Z8" s="13" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+        <v>303</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="L9" s="20" t="s">
-        <v>296</v>
-      </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="O9" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="P9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="R9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="S9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="V9" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="W9" s="1">
         <v>25000</v>
@@ -3609,75 +3748,90 @@
         <v>25</v>
       </c>
       <c r="Z9" s="13" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB9" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="J10" s="3" t="s">
+      <c r="K10" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="M10" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L10" s="20" t="s">
-        <v>296</v>
-      </c>
-      <c r="M10" s="5" t="s">
+      <c r="N10" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="N10" s="6" t="s">
+      <c r="O10" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="P10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q10" s="1" t="s">
+      <c r="R10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="S10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T10" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="W10" s="1">
         <v>25000</v>
@@ -3689,75 +3843,90 @@
         <v>25</v>
       </c>
       <c r="Z10" s="13" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+      <c r="AA10" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB10" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="J11" s="3" t="s">
+      <c r="K11" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="L11" s="20" t="s">
-        <v>296</v>
-      </c>
-      <c r="M11" s="1" t="s">
+      <c r="N11" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="N11" s="6" t="s">
+      <c r="O11" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="P11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T11" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="R11" s="1" t="s">
+      <c r="U11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="S11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="T11" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="V11" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W11" s="1">
         <v>25000</v>
@@ -3769,7 +3938,117 @@
         <v>25</v>
       </c>
       <c r="Z11" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W12" s="1">
+        <v>25000</v>
+      </c>
+      <c r="X12" s="1">
+        <v>35000</v>
+      </c>
+      <c r="Y12" s="6">
+        <v>25</v>
+      </c>
+      <c r="Z12" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>